<commit_message>
small changes variables after pilot
</commit_message>
<xml_diff>
--- a/_static/global/groups_scores.xlsx
+++ b/_static/global/groups_scores.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chbuschi\PycharmProjects\groupmemory\_static\global\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chbuschi\Documents\Research\Group Memory\Otree\Memory\_static\global\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5170E29-01CC-45DC-A417-216048A033F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D320EFD4-FB70-49D3-BE89-9D1A3B4FEED0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="26">
   <si>
     <t>ID</t>
   </si>
@@ -108,6 +108,12 @@
   </si>
   <si>
     <t>663fd4d1ba4f382b5bab924e</t>
+  </si>
+  <si>
+    <t>6687bfc6b173fbe99a38cfb4</t>
+  </si>
+  <si>
+    <t>667ee4bc53bc8bcecb7843a9</t>
   </si>
 </sst>
 </file>
@@ -434,10 +440,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -503,7 +509,7 @@
         <v>8</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F17" si="0">D3+E3</f>
+        <f t="shared" ref="F3:F19" si="0">D3+E3</f>
         <v>8</v>
       </c>
     </row>
@@ -799,6 +805,48 @@
       <c r="F17">
         <f t="shared" si="0"/>
         <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18">
+        <v>2</v>
+      </c>
+      <c r="D18">
+        <v>3</v>
+      </c>
+      <c r="E18">
+        <v>6</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19">
+        <v>2</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19">
+        <v>4</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="0"/>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>